<commit_message>
made it work for multiple urls and not detect blank lines as urls
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,72 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ΠΑΠΑΔΑΚΗΣ ΠΑΥΛΟΣ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Θεσσαλονίκης 160, Πλησίον Ηλεκτρικού Σταθμού, Αθήνα - Κάτω Πετράλωνα, 11853, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Κλινική Δερματολογία - Αφροδισιολογία</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2103455493</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6932351230</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>pavderm@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ΠΙΝΙΩΤΗ Γ. ΠΑΝΑΓΙΩΤΑ MD</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Αγ. Τρύφωνος 22, Γλυφάδα, 16561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Άγχος – Φοβίες - Κατάθλιψη – Κρίσεις Πανικού - Διαταραχές Μνήμης - Διαταραχές Ύπνου - Άνοια - Ψυχωσική Συνδρομή - Ψυχώσεις -  Πένθος  - Διαταραχές Διάθεσης - Συμβουλευτική - Ψυχοθεραπεία - Πιστοποιητικά Ψυχικής Υγείας - Ψυχολογική Υποστήριξη</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6976973323</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://drpinioti.gr/</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>panagiotapinioti@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
removed duplicates and idk
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,97 +469,371 @@
           <t>Email</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ωρες</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ΛΟΥΚΑΣ ΑΝΑΣΤΑΣΙΟΣ PHD</t>
+          <t>ATHENS DENTAL PROJECT - ΜΠΟΥΛΝΤΗΣ ΓΙΩΡΓΟΣ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Σύρου 9-11, Παλαιό τέρμα, Γαλάτσι, 11147, ΑΤΤΙΚΗΣ</t>
+          <t>Λεωφόρος Βουλιαγμένης 604 &amp; Υμηττού 1, Ελληνικό, 16777, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>2102930460</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6944281772</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>Οδοντιατρικό Κέντρο - Χειρουργός Οδοντίατρος - Γενική Οδοντιατρική - Ορθοδοντική</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2111196707</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>6978507450</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>http://athensdentalproject.gr</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>mailTo:anastasiosloukas@gmail.com</t>
-        </is>
-      </c>
+          <t>mailTo:info@athensdentalproject.gr</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ΤΣΟΛΑΚΗΣ ΔΗΜΗΤΡΗΣ</t>
+          <t>MODERN DENTAL CENTER -ΑΧΙΛΛΑΔΕΛΗΣ ΑΓΓΕΛΟΣ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Υπολοχαγού Καββαθά 2, Ζωγράφος, 15773, ΑΤΤΙΚΗΣ</t>
+          <t>Λευκάδος 3, Γλυκά Νερά, 15354, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Παθολόγος – Κατ’ Οίκον Επισκέψεις – Πιστοποιητικά Υγείας - Σύμβαση με Υπουργείο Συγκοινωνιών για Εξέταση Υποψηφίων Οδηγών –  Άυλη Συνταγογράφηση – Γρίπη – Λοιμώξεις Ουροποιητικού – Λοιμώξεις Αναπνευστικού – Πυρετός – Αναιμία – Ουρικό Οξύ – Αρτηριακή Υπέρταση – Δυσλιπιδαιμία – Σακχαρώδης Διαβήτης</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2107774215</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6949529354</v>
+          <t>Χειρουργός Οδοντίατρος - Σύγχρονο Οδοντιατρικό Κέντρο – Περιοδοντολογία  Ενδοδοντία - Προσθετική &amp; Επανορθωτική Οδοντιατρική – Εμφυτεύματα - Γναθοπροσωπική Χειρουργική - Ορθοδοντική Παιδιών &amp; Ενηλίκων -Παιδοδοντιατρική</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2106659317</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6974433659</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://pathologos-tsolakis.gr</t>
+          <t>http://www.moderndental.gr</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>mailTo:dimitrios.tsolakis@gmail.com</t>
-        </is>
-      </c>
+          <t>mailTo:achilladelis@gmail.com</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ΓΕΡΟΝΤΙΔΗ ΟΛΓΑ</t>
+          <t>ΠΡΑΣΣΑ ΑΛΕΞΑΝΔΡΟΥ ΑΝΑΣΤΑΣΙΑ - ΜΑΡΙΑ DR. MED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Λ. Αμαρουσίου 15, Λυκόβρυση, 14123, ΑΤΤΙΚΗΣ</t>
+          <t>Λ. Σουνίου 38, ισόγειο, Μαρκόπουλο, 19003, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Χειρουργός Οδοντίατρος</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2102812023</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6932222192</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>mailTo:gerontidou@gmail.com</t>
-        </is>
-      </c>
+          <t>Χειρουργός Οδοντίατρος Εξειδικευθείς Στην Στοματολογία &amp; Περιοδοντολογία</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6936730545</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>http://www.stomatomed.gr</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DC ORTHODONTIST - ΧΑΡΑΛΑΜΠΟΠΟΥΛΟΥ ΔΗΜΗΤΡΑ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Πλαταιών 2, Πλησίον σταθμού ΗΣΑΠ, Μαρούσι, 15124, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2108055993</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6932756465</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.dcorthoclinic.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>mailTo:dcortho@outlook.com</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ΚΑΚΛΑΜΑΝΗΣ ΑΓΓΕΛΟΣ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Θηβών 210, Περιστέρι, 12134, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Οδοντιατρική Κλινική - Προσθετική - Ενδοδοντία – Γναθοχειρουργική - Ορθοδοντική</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2105730784</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>mailTo:kaklamanisdentalcare@gmail.com</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SPECIALIZED DENTISTRY OF ATHENS - ΛΩΛΗΣ Θ. ΧΡΗΣΤΟΣ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ψυχάρη 1 &amp; Στρατήγη, Φάρος, Νέο Ψυχικό, 15451, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Αισθητική Οδοντιατρική - Εμφυτευματολογία - Προσθετική - Παιδοδοντία - Περιοδοντολογία - Ορθοδοντική</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2106741600</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6974631121</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>http://www.athensdentistry.gr</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>mailTo:sda@athensdentistry.gr</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ΟΔΟΝΤΙΑΤΡΙΚΟ ΚΕΝΤΡΟ ΠΑΛΑΙΟΥ ΦΑΛΗΡΟΥ - ΜΑΡΙΝΑΚΗΣ ΜΑΥΡΟΜΜΑΤΗ ΣΙΑΜΕΤΗ Ο.Ε</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Βενιζέλου Ελευθερίου 186, Παλαιό Φάληρο, 17563, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Το Οδοντιατρικό Κέντρο Παρέχει Υπηρεσίες Που Αφορούν Σε Αισθητική Οδοντιατρική - Λεύκανση – Εμφυτεύματα – Προσθετική - Ενδοδοντικές &amp; Περιοδοντικές Θεραπείες - Παιδοδοντία - Ορθοδοντική</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2109819100</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>6937303142</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://dentalclinicpaliofaliro.gr/</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>mailTo:dentalclinicps@yahoo.com</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ΚΟΤΙΝΑΣ ΑΝΑΣΤΑΣΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Μεσογείων 3, 2ος όροφος, Αθήνα - Αμπελόκηποι, 11526, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2107755320</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>6944636060</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>http://www.akotinas.gr</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>mailTo:akotinas@otenet.gr</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ODOUS MEDICA ΒΑΡΔΑΚΑΣΤΑΝΗ ΑΘΗΝΑ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Καραϊσκάκη 124, Γλυκά Νερά, , ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Λεύκανση - Εμφυτεύματα – Ενδοδοντία – Περιοδοντολογία – Προσθετική - Εμφράξεις</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2106041190</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6950568710</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>http://www.avardakastani.gr</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>mailTo:v.k.athina@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ΜΑΚΡΗΣ ΛΕΩΝΙΔΑΣ</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Πανόρμου 119, 2ος όροφος, Αθήνα - Αμπελόκηποι, 11524, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ενδοδοντολόγος - Περιοδοντολόγος - Χειρουργική Στόματος - Χειρουργική Εξαγωγή Φρονιμιτών - Δεκάλεπτη Λεύκανση Δοντιών Με Laser - Καθαρισμός Δοντιών</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6944594547</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>http://www.odontiatros-makris.gr</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>mailTo:leonmakris@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
i think that recognizes non websites and does the appending correctly
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,105 +461,1455 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Website</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Ωρα</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ΛΟΥΚΑΣ ΑΝΑΣΤΑΣΙΟΣ PHD</t>
+          <t>ΓΙΩΤΗ ΑΙΚΑΤΕΡΙΝΗ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Σύρου 9-11, Παλαιό τέρμα, Γαλάτσι, 11147, ΑΤΤΙΚΗΣ</t>
+          <t>Λυκούργου 104, Σπάρτη, 24133, ΛΑΚΩΝΙΑΣ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
+          <t>Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Χειρουργός Κεφαλής &amp; Τραχήλου - Ακοολογικός Έλεγχος Ενηλίκων &amp; Παιδιών - Ενδοσκοπικός Έλεγχος Ανώτερου Αναπνευστικού &amp; Καταγραφή Της Εξέτασης Σε Video - Διερεύνηση Βαρηκοΐας – Εμβοών – Ιλίγγου – Βραχνάδας - Δυσχέρειας Ρινικής Αναπνοής - Τραχηλικών Διογκώσεων</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2102930460</v>
+        <v>2731026620</v>
       </c>
       <c r="E2" t="n">
-        <v>6944281772</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>6974754853</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mailTo:gioti.orl@gmail.com</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>mailTo:anastasiosloukas@gmail.com</t>
+          <t>na steilw mail me thn doyuleia mou</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ΤΣΟΛΑΚΗΣ ΔΗΜΗΤΡΗΣ</t>
+          <t>ΑΤΖΕΜΙΔΑΚΗΣ ΓΙΩΡΓΟΣ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Υπολοχαγού Καββαθά 2, Ζωγράφος, 15773, ΑΤΤΙΚΗΣ</t>
+          <t>Λουίζης Ριανκούρ 54, Αθήνα - Αμπελόκηποι, 11523, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Παθολόγος – Κατ’ Οίκον Επισκέψεις – Πιστοποιητικά Υγείας - Σύμβαση με Υπουργείο Συγκοινωνιών για Εξέταση Υποψηφίων Οδηγών –  Άυλη Συνταγογράφηση – Γρίπη – Λοιμώξεις Ουροποιητικού – Λοιμώξεις Αναπνευστικού – Πυρετός – Αναιμία – Ουρικό Οξύ – Αρτηριακή Υπέρταση – Δυσλιπιδαιμία – Σακχαρώδης Διαβήτης</t>
+          <t>Χειρουργός Ουρολόγος - Ανδρολόγος</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2107774215</v>
+        <v>2155309555</v>
       </c>
       <c r="E3" t="n">
-        <v>6949529354</v>
+        <v>6947695629</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://pathologos-tsolakis.gr</t>
+          <t>mailTo:atzemidakis.giorgos@gmail.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>mailTo:dimitrios.tsolakis@gmail.com</t>
+          <t>πεμπτη τηλ 3.00 για ραντεβου από κοντα/από σεπτ</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ΓΕΡΟΝΤΙΔΗ ΟΛΓΑ</t>
+          <t>ΑΝΑΣΤΑΣΑΚΗΣ ΔΗΜΟΣΘΕΝΗΣ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Λ. Αμαρουσίου 15, Λυκόβρυση, 14123, ΑΤΤΙΚΗΣ</t>
+          <t>Άννινου Μπάμπη 10Α, Αθήνα, 11144, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Χειρουργός Οδοντίατρος</t>
+          <t>Χειρουργός Ορθοπεδικός - Αθλητικές Κακώσεις – Αρθροσκόπηση - Ορθοπεδική Παιδιών – Τραυματολόγος – Ισχίο – Θλάση – Κάταγμα – Οστεοπόρωση – Αυχενικό – Γόνατο – Superpath - Almis</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2102812023</v>
+        <v>2130333815</v>
       </c>
       <c r="E4" t="n">
-        <v>6932222192</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>mailTo:gerontidou@gmail.com</t>
-        </is>
-      </c>
+        <v>6944744724</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>mailTo:diansgr@hotmail.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ΚΟΝΤΟΥ ΙΩΑΝΝΑ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Λ. Μαραθώνος 27, Πικέρμι, 19009, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Παιδίατρος</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2106036036</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6974121315</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>mailTo:ioannakontou@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ΓΙΑΝΝΟΥΛΗ ΓΕΩΡΓΙΑ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Δημαρχείου 8, μετρό Αιγάλεω Εσταυρωμένος, Αιγάλεω, 12242, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Κλινική Δερματολογία – Αφροδισιολογια - Δερματοχειρουργική - Αισθητική Δερματολογία</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2105902059</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>mailTo:gfg1905@gmail.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ΑΝΔΡΙΝΟΣ ΔΗΜΗΤΡΗΣ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ιωσήφ των Ρωγών 1 &amp; Αθανασίου Διάκου, στάση μετρό Ακρόπολη, Μακρυγιάννη, Αθήνα, 11743, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ψυχίατρος - Ψυχοθεραπευτής</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2130316283</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6943828282</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>mailTo:dimandrinos@gmail.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ΑΝΤΩΝΟΠΟΥΛΟΥ Κ. ΖΩΗ M.D</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Αφροδίτης 47-49 &amp; Αγίου Αλεξάνδρου, Παλαιό Φάληρο, 17561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Χειρουργός Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Επιμελήτρια Τμήματος  Χειρουργικής Τραχήλου Θυρεοειδούς ΩΡΛ Κλινικής Μητέρα</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2109840078</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6977202619</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>mailTo:zoiantonopoulou@gmail.com</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ΓΕΩΡΓΑΚΟΠΟΥΛΟΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ιλίου 33, Ίλιον, 13122, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Παθολόγος – Οικογενειακός Ιατρός Συμβεβλημένος με ΕΟΠΥΥ – Υπέρταση – Διαβήτης – Λοιμώξεις Αναπνευστικού – Check Up - Οστεοπόρωση – Δυσλιπιδαιμία – Χρόνια Νοσήματα</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2105767889</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6973492279</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1.3/πηρα 2 φορες δεν απαντησε</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ΔΗΜΗΤΡΙΟΥ ΚΩΝΣΤΑΝΤΙΝΑ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Σούτσου Δημητρίου 48, Αθήνα - Αμπελόκηποι, 11521, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ενδοκρινολόγος</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2106982208</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6944911408</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>mailTo:konstantina.dimitriou@outlook.com</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ΑΝΤΩΝΟΠΟΥΛΟΣ ΠΑΝΤ. ΑΝΔΡΕΑΣ ΔΡ.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>25ης Μαρτίου 79, Πετρούπολη, 13231, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2105025268</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6972070111</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>mailTo:andon_andreas@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ΑΓΑΠΙΟΥ ΦΩΤΕΙΝΗ</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Λ. Ειρήνης 28, Πεύκη, 15121, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ειδικός Καρδιολόγος – Πιστοποιημένη με ΕΟΠΥΥ Μόνο για Ηλεκτρονική Συνταγογράφηση - Καρδιολογικός Έλεγχος - Triplex Καρδιάς - Αρρυθμίες - Καρδιογράφημα - Test Κοπώσεως - Holter Πίεσης - Check Up</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2106148852</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6987578684</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>mailTo:foteiniagapiou@gmail.com</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>ΘΑ ΚΑΛΕΣΕΙ ΕΚΕΙΝΗ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ΒΟΥΔΟΥΡΗ ΝΙΚΗ MD MSc</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Μαυρομματαίων 31, 250 μ. από Σταθμό Βικτώρια, Αθήνα - Πεδίο Άρεως, 10434, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Παιδοψυχίατρος MD Msc - Διάγνωση Νευροαναπτυξιακών Διαταραχών -  Συναισθηματικές Διαταραχές - Διάσπαση Προσοχής - Συνταγογράφηση Γνωματεύσεων ΕΟΠΥΥ - Προβλήματα Συμπεριφοράς</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2114013841</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6932441469</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>mailTo:nickyvoudouri@gmail.com</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ΑΝΑΣΤΑΣΟΠΟΥΛΟΣ ΑΝΔΡΕΑΣ</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Επιδαύρου 30 &amp; Μαυρομιχαλαίων 8, Χαλάνδρι, 15233, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Πνευμονολόγος - Φυματιολόγος - Msc στην Ογκολογία Θώρακος</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2105713710</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6945404806</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>mailTo:andreas-anastasopoulos@hotmail.com</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ΒΟΥΡΕΞΑΚΗ ΜΑΡΙΝΑ</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Φορμίωνος 36, Αθήνα - Παγκράτι, 11634, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Χειρουργός Οφθαλμίατρος</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2107222551</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6972503355</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>mailTo:mvour@otenet.gr</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ΒΑΛΒΗΣ ΠΑΝΑΓΙΩΤΗΣ</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Λεωφόρος Αθηνών 8, Αχαρνές, 13671, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Χειρουργός Ορθοπεδικός &amp; Χειρουργός Αθλητικών Κακώσεων -  Χειρουργική Ρομποτική</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2114180300</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6932225937</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>mailTo:valvispan@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ΓΟΝΙΔΑΚΗΣ ΑΝΤΩΝΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Αγίας Λαύρας 24, Αιγάλεω, 12244, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ορθοπαιδικός – Χειρουργός – Τραυματιολόγος – Χειροθεραπεία – Οστεοπαθητική</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2105905460</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6936988762</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>mailTo:gonidakis@gmx.de</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ΔΕΒΕΡΑΚΗΣ ΤΙΤΟΣ</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Αριστοτέλους 166 &amp; Πάρνηθος, 1ος όροφος, Αχαρνές, 13674, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Χειρουργός Ουρολόγος – Ανδρολόγος - Στρατιωτικός Ιατρός</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2102406299</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6942076290</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>mailTo:deverakis.urology@gmail.com</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ΒΑΣΙΛΟΠΟΥΛΟΣ Χ. ΙΩΑΝΝΗΣ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Μανουτίου Άλδου 2 - 6, Αθήνα - Αμπελόκηποι, 11521, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Ιατρός ΕΛ.ΑΣ. - Πιστοποιημένος για Ηλεκτρονική Συνταγογράφηση</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2106922953</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6945647623</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>mailTo:vasilopoulosioannis@yahoo.com</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ΓΑΣΠΑΡΙΔΟΥ ΜΑΡΙΑ</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Καλλιρρόης 45, Στάση Μετρό Συγγρού - Φιξ, Αθήνα - Νέος Κόσμος, 11743, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ψυχίατρος - Ιδιωτικό Ιατρείο</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2109248838</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6972202914</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>mailTo:maria.gasparidou1@gmail.com</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ΠΑΠΑΔΑΚΗΣ ΠΑΥΛΟΣ</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Θεσσαλονίκης 160, Πλησίον Ηλεκτρικού Σταθμού, Αθήνα - Κάτω Πετράλωνα, 11853, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Κλινική Δερματολογία - Αφροδισιολογία</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2103455493</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6932351230</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>mailTo:pavderm@gmail.com</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ΑΝΟΜΙΤΡΗ ΧΡΥΣΑΝΘΗ</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Βορείου Ηπείρου 139, Γλυφάδα, 16562, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Παιδοψυχίατρος</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2109645820</v>
+      </c>
+      <c r="E22" t="n">
+        <v>6942820500</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>mailTo:chryna.sun@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ΓΚΟΝΗ ΓΕΩΡΓΙΑ</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Λ. Ηρώων Πολυτεχνείου 75, Πειραιάς, 18536, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ρευματολόγος - Επιστημονικός Συνεργάτης ΕΡΡΙΚΟΣ ΝΤΥΝΑΝ - Γ' Παθολογική Κλινική</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2104111821</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6944722872</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>mailTo:georgia.gkoni@ymail.com</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ΘΑ ΚΑΛΕΣΕΙ ΕΚΕΙΝΗ/εστειλε μηνυμα θα παρει εκεινη</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MICROBIOMEDICA - ΣΜΑΡΓΙΑΝΑΚΗΣ ΘΕΟΔΟΣΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Χρυσοστόμου Σμύρνης 6 &amp; Μάντικα Χρήστου, Ραφήνα, 19009, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Διάγνωση –  Έρευνα –  Πρόληψη</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2294023771</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6936608099</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>mailTo:microbiomedica.lab@gmail.com</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>ΘΑ ΚΑΛΕΣΕΙ ΕΚΕΙΝΟΣ/Από σεπτ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ΚΟΝΤΟΥ ΦΩΤΕΙΝΗ</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Κανάρη 9, Αθήνα - Κολωνάκι, 10673, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ψυχίατρος - Ψυχοθεραπεύτρια - Σύμβουλος Ψυχίατρος Μαιευτηρίου ΙΑΣΩ</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2103622319</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6944962722</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>mailTo:kontoufotini@hotmail.com</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ΑΘΑΝΑΣΙΟΥ Α. ΚΩΝΣΤΑΝΤΙΝΑ</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Τραλλέων 67, Γαλάτσι, 11146, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Χειρουργός Οφθαλμίατρος - Συνεργάτης Θεραπευτηρίου Metropolitan</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2102917955</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6974533639</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>mailTo:kathanasiou.eye@gmail.com</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>ΑΡΧΙΖΩ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ΜΕΘΕΝΙΤΗ ΣΩΤΗΡΙΑ ΣΟΝΙΑ</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Λ. Κηφισίας 341, Κηφισιά, 14561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Οδοντίατρος - Παιδοδοντίατρος</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2108079921</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6944698898</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>mailTo:soniamet@otenet.gr</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>από σεπτεμβρη</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Βογιατζάκης Εμμανουήλ Ν.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ζωοδόχου Πηγής 4, Χαλάνδρι - Κάτω Χαλάνδρι, 15231, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2106753795</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6974484918</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ΦΩΤΟΥΧΟΥ ΕΣΦΑΝΤΙΑΡΙ ΑΛΕΞΑΝΔΡΑ</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Μπουμπουλίνας 51, Νέο Ψυχικό, 15451, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Γενικός Ιατρός – Παθολόγος - Γηρίατρος – Γεροντολόγος - Wheelchair Accessible</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2106745205</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6980351683</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>mailTo:alexandra.esfandiari@gmail.com</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Γρημάη Γεωργία - Μυρσίνη Α.</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ρούσου Χούρδου 8, Ηράκλειο - Πλατεία Δασκαλογιάννη, 71201, ΗΡΑΚΛΕΙΟΥ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2810220570</v>
+      </c>
+      <c r="E30" t="n">
+        <v>6947328410</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Καλλίρη Μπετίνα Π.</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ποταμού Καλαμά 28, Χαλάνδρι, 15233, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2106890513</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Καγκελάρης Νικόλαος Α.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Αριστοφάνους 16, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2106834141</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Μπούτικα Δήμητρα Ε.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Βριλησσίων 26 &amp; Πάροδος Αττικής Οδού, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2106000611</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ΤΡΙΑΝΤΑΦΥΛΛΟΣ Α. ΜΑΝΟΥΣΟΣ - DOCTOR PLUS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Θαλή Μιλησίου 13, Νέα Ερυθραία, 14671, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Επισκέψεις κατ’ οίκον Ηλεκτροκαρδιογραφήματος - Τοποθέτηση Καθετήρων Αναρρόφησης Εκκρίσεων - 'Ελεγχος Κολοστομίας Τραχειοστομίας - Ενδοφλέβια Ένεση - Ενδοφλέβια ΧορΉγηση Φαρμάκων Μέσω Άλλου Φλεβοκαθετήρα</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2108002495</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6977325007</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>mailTo:mdmanousos@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Κατσάκου Δήμητρα Σ.</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Λεωφόρος Πεντέλης 22, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2106856106</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>πεμπτη πρωι(κατά της 12)/ΜΗΝ ΞΑΝΑΠΑΡΩ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ΦΑΣΙΑΝΟΣ ΜΑΡΙΝΟΣ</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Διάκου Αθανασίου 37, Νέα Ερυθραία, 14671, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος Στρατιωτικός Ιατρός</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2107717107</v>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>mailTo:mfasianos@gmail.com</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>τεταρτη πρωι(11.30-12.00)/πηρα ειπε θα παρει εκεινος</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Πέρπερας Αντώνιος Α.</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Όθωνος 8, Χαλάνδρι, 15231, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2106746264</v>
+      </c>
+      <c r="E37" t="n">
+        <v>6941499153</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ΤΖΑΜΟΥΡΑΝΗΣ ΔΗΜΗΤΡΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Φιλίππου Λίτσα 34, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Διδάκτωρ Πανεπιστημίου Αθηνών - Μέλος Ελληνικής Εταιρείας Υπέρτασης - Πιστοποιημένος Ιατρός Στην Ηλεκτρονική Συνταγογράφηση - Σύμβαση Με Υπουργείο Μεταφορών &amp; Ταμείο Τραπέζης Ελλάδος ΑΤΠΣΥΤΕ</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2106838647</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6972246373</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>mailTo:ditzamouranis@gmail.com</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Κωταντούλα Γεωργία</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Κόδρου 22, Εντός Παιδοδοντιατρικής Φροντίδας, Χαλάνδρι, 15231, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2106756420</v>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ΜΑΝΤΖΟΥΚΗΣ ΔΗΜΟΣΘΕΝΗΣ</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Στρατηγού Δαγκλή 157, Αθήνα - Κάτω Πατήσια, 11145, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2108311063</v>
+      </c>
+      <c r="E40" t="n">
+        <v>6974115341</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>mailTo:dimosthenismantzoukis@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Πυλαρινού Στυλιανή Θ.</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Αρκαδίου 38, Χαλάνδρι, 15231, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2106754422</v>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Σοφιανοπούλου - Στίνγκου Μαρία Ι.</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Ηρακλείτου 38, Χαλάνδρι, 15235, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2106000757</v>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Καραμαλίκη Ελίνα Δ.</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Λεωφόρος Κηφισίας 324Α &amp; Αιγαίου 43, Χαλάνδρι, 15233, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2106826514</v>
+      </c>
+      <c r="E43" t="n">
+        <v>6944281011</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>ΠΑΡΑΣΚΕΥΗ ΜΕΤΑ ΤΙΣ 3 Η ΤΗΛΕΦΩΝΙΚΩΣ Η ΑΠΌ ΚΟΝΤΑ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Γκαβάκος Κωνσταντίνος Γ.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Εθνικής Αντιστάσεως 65, Χαλάνδρι, 15231, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2106724944</v>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>μιλησα, από σεπτεμβριο ειπε</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ΚΑΤΣΙΓΙΑΛΟΥ ΝΙΚΗ DDS MSc</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Δεληγιάννη 3, κέντρο, Μεταμόρφωση, 14452, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός - Ορθοδοντική Παιδιών &amp; Ενηλίκων - Invisalign - Αόρατοι Νάρθηκες - Γλωσσικά Σιδεράκια - Προ-Ορθοδοντική - Μασελάκια</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2102838196</v>
+      </c>
+      <c r="E45" t="n">
+        <v>6978875087</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>mailTo:katsigialou.niki@gmail.com</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>από σεπτεμβριο</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ΕΠΙΤΡΟΠΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Λ. Ηρακλείου 366, Νέο Ηράκλειο, 14122, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός Παίδων &amp; Ενηλίκων - DMD - MOrth - Γερμανία - Ηνωμένο Βασίλειο</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2102843353</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>mailTo:dr_epitropakis@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Τριχίλη Αντιγόνη Ε.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Στρατάρχου Παπάγου Αλεξάνδρου 10, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2106817624</v>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ΧΡΙΣΤΑΚΗ ΣΟΦΙΑ</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Αγίας Παρασκευής 9-11, Χαλάνδρι, 15234, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Ειδική Παθολόγος – Επιμελήτρια Παθολόγος Κλινικής Παθολογίας &amp; Ανοσολογίας Της Ευρωκλινικής Αθηνών</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2106835741</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6945592521</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ΚΩΣΤΑΛΑΣ ΛΕΩΝΙΔΑΣ</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>25ης Μαρτίου 3, Χολαργός, 15561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Διδάκτωρ Δημοκρίτειου Πανεπιστήμιου Θράκης - Κατ' Οίκον Επισκέψεις</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2106515029</v>
+      </c>
+      <c r="E49" t="n">
+        <v>6948087946</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>mailTo:ldcostal@gmail.com</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ΜΙΧΟΣ ΠΕΤΡΟΣ</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Μενελάου 138, Ίλιον, 13122, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Χειρουργός Οδοντίατρος – Ορθοδοντική – Γναθοχειρουργική – Εμφυτεύματα – Ενδοδοντία – Περιοδοντολογία – Χειρουργική Στόματος - Λεύκανση Δοντιών – Αισθητική Οδοντιατρική – Λεύκανση Δοντιών – Καθαρισμός Δοντιών – Νάρθηκες Δοντιών</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2102690110</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>6944576573</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>mailTo:mixos.petros@yahoo.gr</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ΦΡΑΓΚΟΥΛΗΣ ΙΩΑΝΝΗΣ</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Ιατρίδου 91, Καλλιθέα, 17675, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Ειδικός Ορθοδοντικός</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2109574728</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>6999574728</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>mailTo:ifortho@otenet.gr</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
at least it deleting in one perasma all the string duplicates not numbers yet
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5625" yWindow="2130" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Φύλλο1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,18 +25,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -46,25 +77,53 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -147,44 +206,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -211,14 +270,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,6 +305,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,166 +317,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -425,13 +462,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.7109375" customWidth="1" min="1" max="1"/>
+    <col width="21.140625" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="3" max="3"/>
+    <col width="19.140625" customWidth="1" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" min="5" max="5"/>
+    <col width="26.85546875" customWidth="1" min="6" max="6"/>
+    <col width="22.42578125" customWidth="1" min="7" max="7"/>
+    <col width="24.85546875" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -464,14 +511,14 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Ωρα</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>ΓΙΩΤΗ ΑΙΚΑΤΕΡΙΝΗ</t>
         </is>
@@ -486,11 +533,15 @@
           <t>Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Χειρουργός Κεφαλής &amp; Τραχήλου - Ακοολογικός Έλεγχος Ενηλίκων &amp; Παιδιών - Ενδοσκοπικός Έλεγχος Ανώτερου Αναπνευστικού &amp; Καταγραφή Της Εξέτασης Σε Video - Διερεύνηση Βαρηκοΐας – Εμβοών – Ιλίγγου – Βραχνάδας - Δυσχέρειας Ρινικής Αναπνοής - Τραχηλικών Διογκώσεων</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>2731026620</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6974754853</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2731026620</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>6974754853</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -504,7 +555,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>ΑΤΖΕΜΙΔΑΚΗΣ ΓΙΩΡΓΟΣ</t>
         </is>
@@ -519,11 +570,15 @@
           <t>Χειρουργός Ουρολόγος - Ανδρολόγος</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>2155309555</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6947695629</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2155309555</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6947695629</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -537,7 +592,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>ΑΝΑΣΤΑΣΑΚΗΣ ΔΗΜΟΣΘΕΝΗΣ</t>
         </is>
@@ -552,21 +607,24 @@
           <t>Χειρουργός Ορθοπεδικός - Αθλητικές Κακώσεις – Αρθροσκόπηση - Ορθοπεδική Παιδιών – Τραυματολόγος – Ισχίο – Θλάση – Κάταγμα – Οστεοπόρωση – Αυχενικό – Γόνατο – Superpath - Almis</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>2130333815</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6944744724</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2130333815</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>6944744724</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>mailTo:diansgr@hotmail.com</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>ΚΟΝΤΟΥ ΙΩΑΝΝΑ</t>
         </is>
@@ -581,21 +639,24 @@
           <t>Παιδίατρος</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>2106036036</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6974121315</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2106036036</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6974121315</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>mailTo:ioannakontou@yahoo.gr</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>ΓΙΑΝΝΟΥΛΗ ΓΕΩΡΓΙΑ</t>
         </is>
@@ -610,19 +671,19 @@
           <t>Κλινική Δερματολογία – Αφροδισιολογια - Δερματοχειρουργική - Αισθητική Δερματολογία</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>2105902059</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2105902059</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>mailTo:gfg1905@gmail.com</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>ΑΝΔΡΙΝΟΣ ΔΗΜΗΤΡΗΣ</t>
         </is>
@@ -637,21 +698,24 @@
           <t>Ψυχίατρος - Ψυχοθεραπευτής</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>2130316283</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6943828282</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2130316283</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6943828282</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>mailTo:dimandrinos@gmail.com</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>ΑΝΤΩΝΟΠΟΥΛΟΥ Κ. ΖΩΗ M.D</t>
         </is>
@@ -666,21 +730,24 @@
           <t>Χειρουργός Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Επιμελήτρια Τμήματος  Χειρουργικής Τραχήλου Θυρεοειδούς ΩΡΛ Κλινικής Μητέρα</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>2109840078</v>
-      </c>
-      <c r="E8" t="n">
-        <v>6977202619</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2109840078</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>6977202619</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>mailTo:zoiantonopoulou@gmail.com</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>ΓΕΩΡΓΑΚΟΠΟΥΛΟΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
         </is>
@@ -695,13 +762,16 @@
           <t>Παθολόγος – Οικογενειακός Ιατρός Συμβεβλημένος με ΕΟΠΥΥ – Υπέρταση – Διαβήτης – Λοιμώξεις Αναπνευστικού – Check Up - Οστεοπόρωση – Δυσλιπιδαιμία – Χρόνια Νοσήματα</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>2105767889</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6973492279</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2105767889</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>6973492279</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>1.3/πηρα 2 φορες δεν απαντησε</t>
@@ -709,7 +779,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>ΔΗΜΗΤΡΙΟΥ ΚΩΝΣΤΑΝΤΙΝΑ</t>
         </is>
@@ -724,21 +794,24 @@
           <t>Ενδοκρινολόγος</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>2106982208</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6944911408</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2106982208</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6944911408</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>mailTo:konstantina.dimitriou@outlook.com</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>ΑΝΤΩΝΟΠΟΥΛΟΣ ΠΑΝΤ. ΑΝΔΡΕΑΣ ΔΡ.</t>
         </is>
@@ -753,21 +826,24 @@
           <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>2105025268</v>
-      </c>
-      <c r="E11" t="n">
-        <v>6972070111</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2105025268</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>6972070111</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>mailTo:andon_andreas@yahoo.gr</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>ΑΓΑΠΙΟΥ ΦΩΤΕΙΝΗ</t>
         </is>
@@ -782,11 +858,15 @@
           <t>Ειδικός Καρδιολόγος – Πιστοποιημένη με ΕΟΠΥΥ Μόνο για Ηλεκτρονική Συνταγογράφηση - Καρδιολογικός Έλεγχος - Triplex Καρδιάς - Αρρυθμίες - Καρδιογράφημα - Test Κοπώσεως - Holter Πίεσης - Check Up</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>2106148852</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6987578684</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2106148852</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>6987578684</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -800,7 +880,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>ΒΟΥΔΟΥΡΗ ΝΙΚΗ MD MSc</t>
         </is>
@@ -815,21 +895,24 @@
           <t>Παιδοψυχίατρος MD Msc - Διάγνωση Νευροαναπτυξιακών Διαταραχών -  Συναισθηματικές Διαταραχές - Διάσπαση Προσοχής - Συνταγογράφηση Γνωματεύσεων ΕΟΠΥΥ - Προβλήματα Συμπεριφοράς</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>2114013841</v>
-      </c>
-      <c r="E13" t="n">
-        <v>6932441469</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2114013841</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>6932441469</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>mailTo:nickyvoudouri@gmail.com</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
         <is>
           <t>ΑΝΑΣΤΑΣΟΠΟΥΛΟΣ ΑΝΔΡΕΑΣ</t>
         </is>
@@ -844,21 +927,24 @@
           <t>Πνευμονολόγος - Φυματιολόγος - Msc στην Ογκολογία Θώρακος</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>2105713710</v>
-      </c>
-      <c r="E14" t="n">
-        <v>6945404806</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2105713710</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>6945404806</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>mailTo:andreas-anastasopoulos@hotmail.com</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>ΒΟΥΡΕΞΑΚΗ ΜΑΡΙΝΑ</t>
         </is>
@@ -873,21 +959,24 @@
           <t>Χειρουργός Οφθαλμίατρος</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>2107222551</v>
-      </c>
-      <c r="E15" t="n">
-        <v>6972503355</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2107222551</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6972503355</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>mailTo:mvour@otenet.gr</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>ΒΑΛΒΗΣ ΠΑΝΑΓΙΩΤΗΣ</t>
         </is>
@@ -902,21 +991,24 @@
           <t>Χειρουργός Ορθοπεδικός &amp; Χειρουργός Αθλητικών Κακώσεων -  Χειρουργική Ρομποτική</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>2114180300</v>
-      </c>
-      <c r="E16" t="n">
-        <v>6932225937</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2114180300</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>6932225937</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>mailTo:valvispan@yahoo.gr</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>ΓΟΝΙΔΑΚΗΣ ΑΝΤΩΝΙΟΣ</t>
         </is>
@@ -931,21 +1023,24 @@
           <t>Ορθοπαιδικός – Χειρουργός – Τραυματιολόγος – Χειροθεραπεία – Οστεοπαθητική</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>2105905460</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6936988762</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2105905460</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>6936988762</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>mailTo:gonidakis@gmx.de</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>ΔΕΒΕΡΑΚΗΣ ΤΙΤΟΣ</t>
         </is>
@@ -960,11 +1055,15 @@
           <t>Χειρουργός Ουρολόγος – Ανδρολόγος - Στρατιωτικός Ιατρός</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>2102406299</v>
-      </c>
-      <c r="E18" t="n">
-        <v>6942076290</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2102406299</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>6942076290</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -976,7 +1075,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
         <is>
           <t>ΒΑΣΙΛΟΠΟΥΛΟΣ Χ. ΙΩΑΝΝΗΣ</t>
         </is>
@@ -991,21 +1090,24 @@
           <t>Ειδικός Παθολόγος - Ιατρός ΕΛ.ΑΣ. - Πιστοποιημένος για Ηλεκτρονική Συνταγογράφηση</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>2106922953</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6945647623</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2106922953</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>6945647623</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>mailTo:vasilopoulosioannis@yahoo.com</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="6" t="inlineStr">
         <is>
           <t>ΓΑΣΠΑΡΙΔΟΥ ΜΑΡΙΑ</t>
         </is>
@@ -1020,21 +1122,24 @@
           <t>Ψυχίατρος - Ιδιωτικό Ιατρείο</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>2109248838</v>
-      </c>
-      <c r="E20" t="n">
-        <v>6972202914</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2109248838</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6972202914</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>mailTo:maria.gasparidou1@gmail.com</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>ΠΑΠΑΔΑΚΗΣ ΠΑΥΛΟΣ</t>
         </is>
@@ -1049,21 +1154,24 @@
           <t>Κλινική Δερματολογία - Αφροδισιολογία</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>2103455493</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6932351230</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2103455493</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>6932351230</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>mailTo:pavderm@gmail.com</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>ΑΝΟΜΙΤΡΗ ΧΡΥΣΑΝΘΗ</t>
         </is>
@@ -1078,21 +1186,24 @@
           <t>Παιδοψυχίατρος</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>2109645820</v>
-      </c>
-      <c r="E22" t="n">
-        <v>6942820500</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2109645820</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>6942820500</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>mailTo:chryna.sun@yahoo.gr</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="7" t="inlineStr">
         <is>
           <t>ΓΚΟΝΗ ΓΕΩΡΓΙΑ</t>
         </is>
@@ -1107,11 +1218,15 @@
           <t>Ρευματολόγος - Επιστημονικός Συνεργάτης ΕΡΡΙΚΟΣ ΝΤΥΝΑΝ - Γ' Παθολογική Κλινική</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>2104111821</v>
-      </c>
-      <c r="E23" t="n">
-        <v>6944722872</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2104111821</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6944722872</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1125,7 +1240,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="7" t="inlineStr">
         <is>
           <t>MICROBIOMEDICA - ΣΜΑΡΓΙΑΝΑΚΗΣ ΘΕΟΔΟΣΙΟΣ</t>
         </is>
@@ -1140,11 +1255,15 @@
           <t>Διάγνωση –  Έρευνα –  Πρόληψη</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>2294023771</v>
-      </c>
-      <c r="E24" t="n">
-        <v>6936608099</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2294023771</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>6936608099</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1158,7 +1277,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="6" t="inlineStr">
         <is>
           <t>ΚΟΝΤΟΥ ΦΩΤΕΙΝΗ</t>
         </is>
@@ -1173,21 +1292,24 @@
           <t>Ψυχίατρος - Ψυχοθεραπεύτρια - Σύμβουλος Ψυχίατρος Μαιευτηρίου ΙΑΣΩ</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>2103622319</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6944962722</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2103622319</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6944962722</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>mailTo:kontoufotini@hotmail.com</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>ΑΘΑΝΑΣΙΟΥ Α. ΚΩΝΣΤΑΝΤΙΝΑ</t>
         </is>
@@ -1202,11 +1324,15 @@
           <t>Χειρουργός Οφθαλμίατρος - Συνεργάτης Θεραπευτηρίου Metropolitan</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>2102917955</v>
-      </c>
-      <c r="E26" t="n">
-        <v>6974533639</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2102917955</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6974533639</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1220,7 +1346,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="4" t="inlineStr">
         <is>
           <t>ΜΕΘΕΝΙΤΗ ΣΩΤΗΡΙΑ ΣΟΝΙΑ</t>
         </is>
@@ -1235,25 +1361,29 @@
           <t>Οδοντίατρος - Παιδοδοντίατρος</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>2108079921</v>
-      </c>
-      <c r="E27" t="n">
-        <v>6944698898</v>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2108079921</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>6944698898</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>mailTo:soniamet@otenet.gr</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>από σεπτεμβρη</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="5" t="inlineStr">
         <is>
           <t>Βογιατζάκης Εμμανουήλ Ν.</t>
         </is>
@@ -1269,17 +1399,19 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>2106753795</v>
-      </c>
-      <c r="E28" t="n">
-        <v>6974484918</v>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2106753795</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>6974484918</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>ΦΩΤΟΥΧΟΥ ΕΣΦΑΝΤΙΑΡΙ ΑΛΕΞΑΝΔΡΑ</t>
         </is>
@@ -1294,21 +1426,24 @@
           <t>Γενικός Ιατρός – Παθολόγος - Γηρίατρος – Γεροντολόγος - Wheelchair Accessible</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>2106745205</v>
-      </c>
-      <c r="E29" t="n">
-        <v>6980351683</v>
-      </c>
-      <c r="F29" t="inlineStr">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2106745205</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6980351683</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>mailTo:alexandra.esfandiari@gmail.com</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="6" t="inlineStr">
         <is>
           <t>Γρημάη Γεωργία - Μυρσίνη Α.</t>
         </is>
@@ -1324,17 +1459,19 @@
           <t>Ειδικός Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>2810220570</v>
-      </c>
-      <c r="E30" t="n">
-        <v>6947328410</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2810220570</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>6947328410</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="5" t="inlineStr">
         <is>
           <t>Καλλίρη Μπετίνα Π.</t>
         </is>
@@ -1350,15 +1487,14 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D31" t="n">
-        <v>2106890513</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2106890513</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="6" t="inlineStr">
         <is>
           <t>Καγκελάρης Νικόλαος Α.</t>
         </is>
@@ -1374,15 +1510,14 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>2106834141</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2106834141</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="6" t="inlineStr">
         <is>
           <t>Μπούτικα Δήμητρα Ε.</t>
         </is>
@@ -1398,15 +1533,14 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>2106000611</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2106000611</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>ΤΡΙΑΝΤΑΦΥΛΛΟΣ Α. ΜΑΝΟΥΣΟΣ - DOCTOR PLUS</t>
         </is>
@@ -1421,21 +1555,24 @@
           <t>Επισκέψεις κατ’ οίκον Ηλεκτροκαρδιογραφήματος - Τοποθέτηση Καθετήρων Αναρρόφησης Εκκρίσεων - 'Ελεγχος Κολοστομίας Τραχειοστομίας - Ενδοφλέβια Ένεση - Ενδοφλέβια ΧορΉγηση Φαρμάκων Μέσω Άλλου Φλεβοκαθετήρα</t>
         </is>
       </c>
-      <c r="D34" t="n">
-        <v>2108002495</v>
-      </c>
-      <c r="E34" t="n">
-        <v>6977325007</v>
-      </c>
-      <c r="F34" t="inlineStr">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2108002495</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>6977325007</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>mailTo:mdmanousos@yahoo.gr</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="7" t="inlineStr">
         <is>
           <t>Κατσάκου Δήμητρα Σ.</t>
         </is>
@@ -1451,19 +1588,19 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D35" t="n">
-        <v>2106856106</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2106856106</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>πεμπτη πρωι(κατά της 12)/ΜΗΝ ΞΑΝΑΠΑΡΩ</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="7" t="inlineStr">
         <is>
           <t>ΦΑΣΙΑΝΟΣ ΜΑΡΙΝΟΣ</t>
         </is>
@@ -1478,23 +1615,24 @@
           <t>Ειδικός Παθολόγος Στρατιωτικός Ιατρός</t>
         </is>
       </c>
-      <c r="D36" t="n">
-        <v>2107717107</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2107717107</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>mailTo:mfasianos@gmail.com</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>τεταρτη πρωι(11.30-12.00)/πηρα ειπε θα παρει εκεινος</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t>Πέρπερας Αντώνιος Α.</t>
         </is>
@@ -1510,17 +1648,19 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>2106746264</v>
-      </c>
-      <c r="E37" t="n">
-        <v>6941499153</v>
-      </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2106746264</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>6941499153</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="6" t="inlineStr">
         <is>
           <t>ΤΖΑΜΟΥΡΑΝΗΣ ΔΗΜΗΤΡΙΟΣ</t>
         </is>
@@ -1535,21 +1675,24 @@
           <t>Ειδικός Παθολόγος - Διδάκτωρ Πανεπιστημίου Αθηνών - Μέλος Ελληνικής Εταιρείας Υπέρτασης - Πιστοποιημένος Ιατρός Στην Ηλεκτρονική Συνταγογράφηση - Σύμβαση Με Υπουργείο Μεταφορών &amp; Ταμείο Τραπέζης Ελλάδος ΑΤΠΣΥΤΕ</t>
         </is>
       </c>
-      <c r="D38" t="n">
-        <v>2106838647</v>
-      </c>
-      <c r="E38" t="n">
-        <v>6972246373</v>
-      </c>
-      <c r="F38" t="inlineStr">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2106838647</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>6972246373</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>mailTo:ditzamouranis@gmail.com</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="5" t="inlineStr">
         <is>
           <t>Κωταντούλα Γεωργία</t>
         </is>
@@ -1565,15 +1708,14 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D39" t="n">
-        <v>2106756420</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2106756420</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="5" t="inlineStr">
         <is>
           <t>ΜΑΝΤΖΟΥΚΗΣ ΔΗΜΟΣΘΕΝΗΣ</t>
         </is>
@@ -1588,21 +1730,24 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D40" t="n">
-        <v>2108311063</v>
-      </c>
-      <c r="E40" t="n">
-        <v>6974115341</v>
-      </c>
-      <c r="F40" t="inlineStr">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2108311063</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>6974115341</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>mailTo:dimosthenismantzoukis@yahoo.gr</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="6" t="inlineStr">
         <is>
           <t>Πυλαρινού Στυλιανή Θ.</t>
         </is>
@@ -1618,15 +1763,14 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D41" t="n">
-        <v>2106754422</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2106754422</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t>Σοφιανοπούλου - Στίνγκου Μαρία Ι.</t>
         </is>
@@ -1642,15 +1786,14 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D42" t="n">
-        <v>2106000757</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2106000757</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>Καραμαλίκη Ελίνα Δ.</t>
         </is>
@@ -1666,21 +1809,24 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D43" t="n">
-        <v>2106826514</v>
-      </c>
-      <c r="E43" t="n">
-        <v>6944281011</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2106826514</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>6944281011</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
         <is>
           <t>ΠΑΡΑΣΚΕΥΗ ΜΕΤΑ ΤΙΣ 3 Η ΤΗΛΕΦΩΝΙΚΩΣ Η ΑΠΌ ΚΟΝΤΑ</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="4" t="inlineStr">
         <is>
           <t>Γκαβάκος Κωνσταντίνος Γ.</t>
         </is>
@@ -1696,19 +1842,19 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D44" t="n">
-        <v>2106724944</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2106724944</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
         <is>
           <t>μιλησα, από σεπτεμβριο ειπε</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="4" t="inlineStr">
         <is>
           <t>ΚΑΤΣΙΓΙΑΛΟΥ ΝΙΚΗ DDS MSc</t>
         </is>
@@ -1723,25 +1869,29 @@
           <t>Ειδικός Ορθοδοντικός - Ορθοδοντική Παιδιών &amp; Ενηλίκων - Invisalign - Αόρατοι Νάρθηκες - Γλωσσικά Σιδεράκια - Προ-Ορθοδοντική - Μασελάκια</t>
         </is>
       </c>
-      <c r="D45" t="n">
-        <v>2102838196</v>
-      </c>
-      <c r="E45" t="n">
-        <v>6978875087</v>
-      </c>
-      <c r="F45" t="inlineStr">
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2102838196</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>6978875087</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>mailTo:katsigialou.niki@gmail.com</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>από σεπτεμβριο</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t>ΕΠΙΤΡΟΠΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
         </is>
@@ -1756,19 +1906,19 @@
           <t>Ειδικός Ορθοδοντικός Παίδων &amp; Ενηλίκων - DMD - MOrth - Γερμανία - Ηνωμένο Βασίλειο</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>2102843353</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2102843353</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>mailTo:dr_epitropakis@yahoo.gr</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="6" t="inlineStr">
         <is>
           <t>Τριχίλη Αντιγόνη Ε.</t>
         </is>
@@ -1784,15 +1934,14 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D47" t="n">
-        <v>2106817624</v>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2106817624</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="5" t="inlineStr">
         <is>
           <t>ΧΡΙΣΤΑΚΗ ΣΟΦΙΑ</t>
         </is>
@@ -1807,17 +1956,19 @@
           <t>Ειδική Παθολόγος – Επιμελήτρια Παθολόγος Κλινικής Παθολογίας &amp; Ανοσολογίας Της Ευρωκλινικής Αθηνών</t>
         </is>
       </c>
-      <c r="D48" t="n">
-        <v>2106835741</v>
-      </c>
-      <c r="E48" t="n">
-        <v>6945592521</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2106835741</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>6945592521</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="5" t="inlineStr">
         <is>
           <t>ΚΩΣΤΑΛΑΣ ΛΕΩΝΙΔΑΣ</t>
         </is>
@@ -1832,86 +1983,1338 @@
           <t>Ειδικός Παθολόγος - Διδάκτωρ Δημοκρίτειου Πανεπιστήμιου Θράκης - Κατ' Οίκον Επισκέψεις</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>2106515029</v>
-      </c>
-      <c r="E49" t="n">
-        <v>6948087946</v>
-      </c>
-      <c r="F49" t="inlineStr">
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2106515029</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>6948087946</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>mailTo:ldcostal@gmail.com</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ΜΙΧΟΣ ΠΕΤΡΟΣ</t>
+          <t>ΨΑΛΤΑΚΟΥ ΜΑΡΙΑ</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Μενελάου 138, Ίλιον, 13122, ΑΤΤΙΚΗΣ</t>
+          <t>Αγίας Βαρβάρας 7, Καλλιθέα, 17676, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Χειρουργός Οδοντίατρος – Ορθοδοντική – Γναθοχειρουργική – Εμφυτεύματα – Ενδοδοντία – Περιοδοντολογία – Χειρουργική Στόματος - Λεύκανση Δοντιών – Αισθητική Οδοντιατρική – Λεύκανση Δοντιών – Καθαρισμός Δοντιών – Νάρθηκες Δοντιών</t>
+          <t>Ειδική Παθολόγος - Οικογενειακή Ιατρός - Ειδικευθείσα Σε Ελβετία - Κατ' Οίκον Επισκέψεις - Συμβεβλημένη με τον ΕΟΠΥΥ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2102690110</t>
+          <t>2109566774</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>6944576573</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>mailTo:mixos.petros@yahoo.gr</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>6970506798</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>mailTo:psaltakoum@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ΦΡΑΓΚΟΥΛΗΣ ΙΩΑΝΝΗΣ</t>
+          <t>ΜΠΑΛΗ ΑΣΗΜΙΝΑ</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ιατρίδου 91, Καλλιθέα, 17675, ΑΤΤΙΚΗΣ</t>
+          <t>Κάτωνος 10, Ηλιούπολη, 16345, ΑΤΤΙΚΗΣ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ειδικός Ορθοδοντικός</t>
+          <t>Παθολόγος - Προσωπικός Γιατρός - Συμβεβλημένη με ΕΟΠΥΥ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2109574728</t>
+          <t>2111158777</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>6999574728</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>mailTo:ifortho@otenet.gr</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>6978222644</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>mailTo:aminabali9747@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ΖΑΡΚΟΥ ΣΤΑΥΡΟΥΛΑ</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Εθνικής Αντιστάσεως 74, Πετρούπολη, 13231, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Σακχαρώδης Διαβήτης – Δυσλιπιδαιμία – Υπέρταση – Λοιμώξεις - Παρακολούθηση Χρόνιων Νοσημάτων - Πρόληψη Καρδιαγγειακών Συμβαμάτων - Συνταγογραφία - Αναγραφή Εξετάσεων Check Up - Χορήγηση Ιατρικών Γνωματεύσεων &amp; Πιστοποιητικών Υγείας - Διερεύνηση Παθήσεων Αγνώστου Αιτιολογίας</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2111181200</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>6981033171</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>mailTo:stavriannazark@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ΚΑΓΚΕΛΑΡΗ Π. ΕΛΕΥΘΕΡΙΑ MD</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Λέκκα Θεοδώρου 9, Αχαρνές, 13673, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Σακχαρώδης Διαβήτης - Αρτηριακή Υπέρταση - Υπερλιπιδαιμία - Λοιμώξεις - Χρόνιες Παθήσεις - Διαφορική Διαγνωστική &amp; Θεραπευτική Παρακολούθηση</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2102449412</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>6974953295</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>mailTo:riak107@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ΗΛΙΑΔΟΥ ΕΛΙΣΑΒΕΤ</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Νικολάου Πλαστήρα 18, Νέα Σμύρνη, 17121, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Εξειδίκευση στον Σακχαρώδη Διαβήτη &amp; την Παχυσαρκία</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2109315648</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>6974345938</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>mailTo:elsa_iliadou@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ΦΛΩΡΟΥ ΣΟΦΙΑ</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Ελ. Βενιζέλου 111, Καλλιθέα, 17672, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2109591846</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>6945857491</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>mailTo:florousofia@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Κατσαδώρου Ελίζα Δ.</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Λεωφόρος Καλάμου 18, Καπανδρίτι, 19014, ΑΤΤΙΚΗΣ
+Δες στον χάρτη</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2295054665</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ΝΤΟΥΝΑ ΚΑΤΕΡΙΝΑ</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Υψηλάντου 138, 2ος όροφος, Πειραιάς, 18535, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Σύμβαση με Υπουργείο Συγκοινωνιών</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2114103647</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>6972838250</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>mailTo:dounakat@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ΣΟΦΟΥΛΗΣ ΝΙΚΟΛΑΟΣ</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Αρχιμήδους 9 &amp; Ξενοφώντος 14, Ηλιούπολη, 16343, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος – Ηπατολόγος – Στρατιωτικός Ιατρός</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2109919010</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>6944414808</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>mailTo:sofoulisn@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ΣΟΥΛΙΩΤΗΣ Α. ΝΙΚΟΛΑΟΣ MD</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Λ. Βάρης 6 &amp; Αγίων Αποστόλων, Βάρη, 16672, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος  – Υπέρταση – Σάκχαρο – Διαβήτης – Λοιμώξεις - Ιώσεις - Ρύθμιση Αρτηριακής Υπέρτασης - Ρύθμιση Σακχάρου - Κατ' Οίκον Επισκέψεις Πιστοποιημένος Για Ηλεκτρονική Συνταγογράφηση &amp; Παρακλινικές Εξετάσεις - Οξυμετρία</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2121053500</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>6937374680</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>mailTo:nik.a.souliotis@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ΣΥΡΜΑΚΕΣΗΣ ΒΑΣΙΛΕΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>25ης Μαρτίου 166 &amp; Ιωάννου Χρυσοστόμου 94, Πετρούπολη, 13231, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Οικογενειακός Ιατρός - Παθολόγος - Επισκέψεις Κατ' Οίκον</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2105014500</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>6977037641</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ΚΟΥΜΠΕΛΗ ΑΝΑΣΤΑΣΙΑ MD</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Διγενή 18, 2oς όροφος, Βούλα, 16673, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Οικογενειακός Γιατρός - Ιδιωτικό Ιατρείο - Πιστοποίηση Για Ηλεκτρονική Συνταγογράφηση Φαρμάκων Και Διαγνωστικών Εξετάσεων Μέσω ΕΟΠΥΥ</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2109658906</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>6932632898</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>mailTo:akoubeli@otenet.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ΚΑΤΣΑΡΑ ΣΤ. ΚΑΡΛΑ - ΙΩΑΝΝΑ MD MSC</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Ευελπίδων 59, Αθήνα - Κυψέλη, 11362, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2108225065</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>6947434884</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>mailTo:carlakts@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ΚΑΡΑΜΠΕΛΑ ΑΡΓΥΡΟΥΛΑ</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Νίκης 9, Νέα Ιωνία - Αλσούπολη, 14235, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2102799540</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>6946369199</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>mailTo:argkarabelamed@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ΚΩΝΣΤΑΝΤΟΠΟΥΛΟΥ ΠΑΝΑΓΙΩΤΑ</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Λ. Γρηγορίου Αυξεντίου 59, Ζωγράφος - Άνω Ιλίσια, 15771, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος Διαβητολόγος - Πιστοποιημένος ιατρός ΕΟΠΥΥ</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2107799566</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>6944654891</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>mailTo:pkonstantopoulou59@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ΑΘΑΝΑΣΟΠΟΥΛΟΥ ΣΤΑΜΑΤΙΑ MD</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Λ. Τσαλδάρη Παναγή 63, Περιστέρι, 12134, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Σακχαρώδης Διαβήτης - Υπέρταση - Ηπατολόγος - Ρύθμιση Λοιμώξεων -Αναιμία - Παχυσαρκία - Προληπτικός Έλεγχος - Επίσκεψη Κατόπιν Ραντεβού &amp; Κατ΄οίκον</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2114081622</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>6947326295</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>mailTo:matinathanas@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ΤΡΙΑΝΤΑΦΥΛΛΟΥ ΒΑΣΙΛΙΚΗ</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Θηβών 137, Περιστέρι, 12136, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Ιατρείο Γενικής Οικογενειακής Ιατρικής - Παροχή Ιατρικής Βοήθειας Στο Σπίτι</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2168081782</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>6945345458</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>mailTo:vastriant30@hotmail.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ΔΟΥΛΓΕΡΑΚΗΣ ΔΗΜΗΤΡΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Ιωαννίνων 5, Γέρακας, 15344, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2106610209</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>6974016795</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>mailTo:gerakasdoctor@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ΜΑΡΗ ΑΝΔΡΙΑΝΑ MD</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Λ. Δημοκρατίας 77, Μελίσσια, 15127, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Στρατιωτικός Ιατρός - Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2111165089</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>6941505426</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>mailTo:annamarh2011@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ΚΑΛΛΟΝΙΑΤΗΣ ΘΕΟΔΩΡΟΣ</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Ανθέων 10, Μαρκόπουλο, 19003, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Οικογενειακός Γιατρός</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2299049199</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>6977695222</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>mailTo:kolkal@hotmail.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ΚΑΡΝΕΖΗ ΚΩΝ/ΝΑ</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Ηρακλείου 425, Νέο Ηράκλειο, 14122, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2102855326</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>6977562551</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>mailTo:kkarnezi@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ΣΑΓΙΑ ΧΑΡΑ MD</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Ηρ. Πολυτεχνείου 62, πλ. Τερψιθέας, Πειραιάς, 18535, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος &amp; Διαιτολόγος</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>6944542221</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>mailTo:sagiahara@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ΜΑΝΕΣΗΣ Κ. ΕΜΜΑΝΟΥΗΛ</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Χέυδεν 1, Πεδίον Άρεως, Αθήνα, 10434, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Ιατρός Ηπατολόγος</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2108829023</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>6974661171</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>mailTo:emanesis@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ΔΡΑΝΔΑΚΗΣ Ε. ΣΟΦΟΚΛΗΣ</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Λεωφ. Ειρήνης 15, Άνωθεν τράπεζας Eurobank, Πεύκη, 15121, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος – Επιμελητής Ιατρικού Ομίλου Αθηνών</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2106124549</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>6942409460</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>mailTo:sofoklisdr@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ΒΙΓΛΑΣ ΒΑΣΙΛΕΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Γεωργίου Γεννηματά 82, Γλυφάδα, 16561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Λοιμωξιολόγος-Επιμελητής Β΄ Παθολογικής - Λοιμωξιολογικής Κλινικής Νοσοκομείου Υγεία - Επισκέψεις Κατ' Οίκον</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2109646114</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>mailTo:billviglas@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ΛΟΥΚΑΣ ΑΝΑΣΤΑΣΙΟΣ PHD</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Σύρου 9-11, Παλαιό τέρμα, Γαλάτσι, 11147, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2102930460</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>6944281772</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>mailTo:anastasiosloukas@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ΧΡΙΣΤΟΔΟΥΛΟΥ ΧΑΡΗΣ</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Μυστρά 50Β, Γλυφάδα, 16561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Παθολόγος - Ιατρός Εργασίας - Βελονιστής – Γενική Τόνωση του Οργανισμού - Παχυσαρκία - Διακοπή Καπνίσματος - Αλλεργίες - Ρευματισμοί - Άγχος -  Εγκεφαλικά Επεισόδια - Μεσοθεραπεία</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2109646400</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>6944348562</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>mailTo:charis.christodoulou@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>ΧΟΥΝΤΗΣ ΔΗΜΗΤΡΗΣ</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Ευγενίου Καραβία 57, πλησίον ΗΣΑΠ, Αθήνα - Κάτω Πατήσια, 11254, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Πιστοποιημένος ΕΟΠΥΥ - Συμβεβλημένος ΕΥΔΑΠ - Θεωρήσεις Διπλωμάτων Οδήγησης - Πιστοποιητικά Υγείας</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2102014314</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>6972190704</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>mailTo:dimitris@olympicnet.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ΠΙΑΓΚΟΣ ΓΙΑΝΝΟΥΛΗΣ</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Κυψέλης 41, Αθήνα - Κυψέλη, 11361, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Γενικός Οικογενειακός Ιατρός - 24 Ώρες Νοσηλεία Και Παροχή Ιατρικής Βοήθειας Στο Σπίτι</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2108830727</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>6979494266</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>mailTo:giannillos@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>ΧΟΥΝΤΗΣ ΔΗΜΗΤΡΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Λ. Κηφισίας 36, έναντι ξενοδοχείου President, Αθήνα - Αμπελόκηποι, 11526, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Πιστοποιημένος ΕΟΠΥΥ - Συμβεβλημένος ΕΥΔΑΠ - Θεωρήσεις Διπλωμάτων Οδήγησης - Πιστοποιητικά Υγείας</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2107482041</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>6972190704</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>ΠΑΝΑΓΙΩΤΑΚΟΠΟΥΛΟΥ ΑΓΓΕΛΙΚΗ MD, PhD</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Ρόδου 13, 1ος όροφος, Μαρούσι, 15122, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Παθολόγος – Αναπληρώτρια Διευθύντρια Β’ Παθολογικής Κλινικής Νοσοκομείου «ΜΗΤΕΡΑ» – Διαβήτης – Λοιμώξεις - Υπερλιπιδαιμία</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2106148114</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>6974492510</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>mailTo:overseas29@msn.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>ΣΔΡΑΚΑ ΕΛΕΝΗ</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Λ. Παπάγου &amp; Μουρκούση Χ. &amp; Α. 2, Ζωγράφος, 15773, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Ανανεώσεις Διπλωμάτων Οδήγησης - Βεβαιώσεις Διπλώματος Οδήγησης - Λοιμώξεις Θεραπεία Αντιμετώπιση - Σακχαρώδης Διαβήτης Υπερλιπιδαιμία - Υπέρταση Έλεγχος - Εξετάσεις Αίματος - Συνταγογράφηση Φαρμάκων - Χρόνια Νοσήματα - Πιστοποιητικά Υγείας - Βεβαιώσεις Θεωρήσεις Διπλωμάτων</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2155255842</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>6973531577</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>mailTo:esdr@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>ΡΑΠΤΗΣ ΑΘΑΝΑΣΙΟΣ</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Αντήνορος 2-4, Αθήνα, 11634, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Διαβητολόγος – Καθηγητής Παθολογίας - Σακχαρώδη Διαβήτη  Ιατρικής Σχολής Πανεπιστημίου - Πιστοποιημένος ΕΟΠΥΥ</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2117350265</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>mailTo:atraptis@med.uoa.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>ΑΝΑΣΤΑΣΑΚΗΣ ΧΡΙΣΤΟΦΟΡΟΣ</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Ευαγγελιστρίας 2 &amp; Σωτηρίου, εντός εμπορικού κέντρου έναντι Εθνικής τράπεζας, Μαρκόπουλο, 19003, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Διαβητικό Πόδι - Σακχαρώδης Διαβήτης &amp; Διατροφή - Αρτηριακή Υπέρταση - Αυξημένα Λιπίδια -Δυσλιπιδαιμία – Εμβολιασμοί - Λοιμώξεις – Αλλεργίες – Οστεοπόρωση - Ψυχοσωματικά Νοσήματα</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2299063249</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>6999440441</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>mailTo:christoforosan@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>ΠΕΤΡΟΥ ΑΛΕΞΑΝΔΡΑ</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>25ης Μαρτίου 154 &amp; Ομήρου 3, Πετρούπολη, 13231, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Παθολόγος - Εξειδίκευση σε Σακχαρώδη Διαβήτη, Διαβητικό Πόδι, Παχυσαρκία</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2105057277</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>6972076641</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>mailTo:alekpetrou@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>ΑΝΑΣΤΑΣΟΠΟΥΛΟΣ ΔΗΜΗΤΡΙΟΣ MD MSc</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Πρωτέως 61, Παλαιό Φάληρο, 17561, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Αναπληρωτής Διευθυντής Παθολογικής Κλινικής Metropolitan General</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2109833368</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>6978061340</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>mailTo:anadim7@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ΠΛΑΤΗΣ Β. ΙΩΑΝΝΗΣ MD</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Ασκληπιού 18, Αθήνα - Κολωνάκι, 10680, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2130231610</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>6977658236</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>mailTo:jplatis@freemail.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>ΓΟΓΑΛΗΣ ΘΕΟΔΩΡΟΣ</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Ατταλείας 225Β, Νίκαια, 18453, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Ιατρός Ειδικός Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2104940317</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>6978613054</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>mailTo:gogalistheodoros@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ΖΑΧΑΡΟΠΟΥΛΟΥ ΡΑΝΙΑ</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Σόλωνος 60, Καλλιθέα, 17673, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2109414967</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>6944900690</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>mailTo:gianira3@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>ΔΑΛΑΚΛΙΔΟΥ ΒΑΣΙΛΙΚΗ</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Βρυαξίδος 12, Αθήνα - Παγκράτι, 11635, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Σύμβαση Με Το Υπουργείο Μεταφορών Για Έκδοση Πιστοποιητικών Υγείας</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2107665604</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>6946246807</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>mailTo:vdalaklidou@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ΦΙΛΗΣ ΧΡΗΣΤΟΣ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Φειδιππίδου 8, Αθήνα - Αμπελόκηποι, 11526, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Παθολόγος</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2107774666</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>6972920788</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>mailTo:christos.filis@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ΚΑΠΡΑΛΟΣ ΧΡΗΣΤΟΣ</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Θεμιστοκλέους 66-68, Περιστέρι, 12134, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Ειδικός Παθολόγος - Εξειδικευθείς σε Υπέρταση - Διακοπή Καπνίσματος - Ηλεκτρονική Συνταγογράφηση μέσω ΕΟΠΥΥ</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>6944197808</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>mailTo:xkapralos5@yahoo.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ΤΡΙΑΝΤΑΦΥΛΛΟΣ Α. ΜΑΝΟΥΣΟΣ - DOCTOR PLUS</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>6977325007</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TELOS TO REMOVE DUPLICATES ITS OK
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Φύλλο1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -464,8 +464,8 @@
   </sheetPr>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -533,15 +533,11 @@
           <t>Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Χειρουργός Κεφαλής &amp; Τραχήλου - Ακοολογικός Έλεγχος Ενηλίκων &amp; Παιδιών - Ενδοσκοπικός Έλεγχος Ανώτερου Αναπνευστικού &amp; Καταγραφή Της Εξέτασης Σε Video - Διερεύνηση Βαρηκοΐας – Εμβοών – Ιλίγγου – Βραχνάδας - Δυσχέρειας Ρινικής Αναπνοής - Τραχηλικών Διογκώσεων</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2731026620</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6974754853</t>
-        </is>
+      <c r="D2" t="n">
+        <v>2731026620</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6974754853</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -570,15 +566,11 @@
           <t>Χειρουργός Ουρολόγος - Ανδρολόγος</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2155309555</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6947695629</t>
-        </is>
+      <c r="D3" t="n">
+        <v>2155309555</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6947695629</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -607,15 +599,11 @@
           <t>Χειρουργός Ορθοπεδικός - Αθλητικές Κακώσεις – Αρθροσκόπηση - Ορθοπεδική Παιδιών – Τραυματολόγος – Ισχίο – Θλάση – Κάταγμα – Οστεοπόρωση – Αυχενικό – Γόνατο – Superpath - Almis</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2130333815</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6944744724</t>
-        </is>
+      <c r="D4" t="n">
+        <v>2130333815</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6944744724</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -639,15 +627,11 @@
           <t>Παιδίατρος</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2106036036</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>6974121315</t>
-        </is>
+      <c r="D5" t="n">
+        <v>2106036036</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6974121315</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -671,10 +655,8 @@
           <t>Κλινική Δερματολογία – Αφροδισιολογια - Δερματοχειρουργική - Αισθητική Δερματολογία</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2105902059</t>
-        </is>
+      <c r="D6" t="n">
+        <v>2105902059</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -698,15 +680,11 @@
           <t>Ψυχίατρος - Ψυχοθεραπευτής</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2130316283</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>6943828282</t>
-        </is>
+      <c r="D7" t="n">
+        <v>2130316283</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6943828282</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -730,15 +708,11 @@
           <t>Χειρουργός Ωτορινολαρυγγολόγος Ενηλίκων &amp; Παίδων - Επιμελήτρια Τμήματος  Χειρουργικής Τραχήλου Θυρεοειδούς ΩΡΛ Κλινικής Μητέρα</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2109840078</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>6977202619</t>
-        </is>
+      <c r="D8" t="n">
+        <v>2109840078</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6977202619</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -762,15 +736,11 @@
           <t>Παθολόγος – Οικογενειακός Ιατρός Συμβεβλημένος με ΕΟΠΥΥ – Υπέρταση – Διαβήτης – Λοιμώξεις Αναπνευστικού – Check Up - Οστεοπόρωση – Δυσλιπιδαιμία – Χρόνια Νοσήματα</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2105767889</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>6973492279</t>
-        </is>
+      <c r="D9" t="n">
+        <v>2105767889</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6973492279</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -794,15 +764,11 @@
           <t>Ενδοκρινολόγος</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2106982208</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>6944911408</t>
-        </is>
+      <c r="D10" t="n">
+        <v>2106982208</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6944911408</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -826,15 +792,11 @@
           <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2105025268</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>6972070111</t>
-        </is>
+      <c r="D11" t="n">
+        <v>2105025268</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6972070111</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -858,15 +820,11 @@
           <t>Ειδικός Καρδιολόγος – Πιστοποιημένη με ΕΟΠΥΥ Μόνο για Ηλεκτρονική Συνταγογράφηση - Καρδιολογικός Έλεγχος - Triplex Καρδιάς - Αρρυθμίες - Καρδιογράφημα - Test Κοπώσεως - Holter Πίεσης - Check Up</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2106148852</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6987578684</t>
-        </is>
+      <c r="D12" t="n">
+        <v>2106148852</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6987578684</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -895,15 +853,11 @@
           <t>Παιδοψυχίατρος MD Msc - Διάγνωση Νευροαναπτυξιακών Διαταραχών -  Συναισθηματικές Διαταραχές - Διάσπαση Προσοχής - Συνταγογράφηση Γνωματεύσεων ΕΟΠΥΥ - Προβλήματα Συμπεριφοράς</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2114013841</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>6932441469</t>
-        </is>
+      <c r="D13" t="n">
+        <v>2114013841</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6932441469</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -927,15 +881,11 @@
           <t>Πνευμονολόγος - Φυματιολόγος - Msc στην Ογκολογία Θώρακος</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2105713710</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>6945404806</t>
-        </is>
+      <c r="D14" t="n">
+        <v>2105713710</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6945404806</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -959,15 +909,11 @@
           <t>Χειρουργός Οφθαλμίατρος</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2107222551</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>6972503355</t>
-        </is>
+      <c r="D15" t="n">
+        <v>2107222551</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6972503355</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -991,15 +937,11 @@
           <t>Χειρουργός Ορθοπεδικός &amp; Χειρουργός Αθλητικών Κακώσεων -  Χειρουργική Ρομποτική</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2114180300</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6932225937</t>
-        </is>
+      <c r="D16" t="n">
+        <v>2114180300</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6932225937</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1023,15 +965,11 @@
           <t>Ορθοπαιδικός – Χειρουργός – Τραυματιολόγος – Χειροθεραπεία – Οστεοπαθητική</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2105905460</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>6936988762</t>
-        </is>
+      <c r="D17" t="n">
+        <v>2105905460</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6936988762</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1055,15 +993,11 @@
           <t>Χειρουργός Ουρολόγος – Ανδρολόγος - Στρατιωτικός Ιατρός</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2102406299</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>6942076290</t>
-        </is>
+      <c r="D18" t="n">
+        <v>2102406299</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6942076290</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1090,15 +1024,11 @@
           <t>Ειδικός Παθολόγος - Ιατρός ΕΛ.ΑΣ. - Πιστοποιημένος για Ηλεκτρονική Συνταγογράφηση</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2106922953</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>6945647623</t>
-        </is>
+      <c r="D19" t="n">
+        <v>2106922953</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6945647623</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1122,15 +1052,11 @@
           <t>Ψυχίατρος - Ιδιωτικό Ιατρείο</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2109248838</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>6972202914</t>
-        </is>
+      <c r="D20" t="n">
+        <v>2109248838</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6972202914</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1154,15 +1080,11 @@
           <t>Κλινική Δερματολογία - Αφροδισιολογία</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2103455493</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>6932351230</t>
-        </is>
+      <c r="D21" t="n">
+        <v>2103455493</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6932351230</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1186,15 +1108,11 @@
           <t>Παιδοψυχίατρος</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2109645820</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>6942820500</t>
-        </is>
+      <c r="D22" t="n">
+        <v>2109645820</v>
+      </c>
+      <c r="E22" t="n">
+        <v>6942820500</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1218,15 +1136,11 @@
           <t>Ρευματολόγος - Επιστημονικός Συνεργάτης ΕΡΡΙΚΟΣ ΝΤΥΝΑΝ - Γ' Παθολογική Κλινική</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2104111821</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>6944722872</t>
-        </is>
+      <c r="D23" t="n">
+        <v>2104111821</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6944722872</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1255,15 +1169,11 @@
           <t>Διάγνωση –  Έρευνα –  Πρόληψη</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2294023771</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>6936608099</t>
-        </is>
+      <c r="D24" t="n">
+        <v>2294023771</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6936608099</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1292,15 +1202,11 @@
           <t>Ψυχίατρος - Ψυχοθεραπεύτρια - Σύμβουλος Ψυχίατρος Μαιευτηρίου ΙΑΣΩ</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2103622319</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>6944962722</t>
-        </is>
+      <c r="D25" t="n">
+        <v>2103622319</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6944962722</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1324,15 +1230,11 @@
           <t>Χειρουργός Οφθαλμίατρος - Συνεργάτης Θεραπευτηρίου Metropolitan</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2102917955</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>6974533639</t>
-        </is>
+      <c r="D26" t="n">
+        <v>2102917955</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6974533639</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1361,15 +1263,11 @@
           <t>Οδοντίατρος - Παιδοδοντίατρος</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2108079921</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>6944698898</t>
-        </is>
+      <c r="D27" t="n">
+        <v>2108079921</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6944698898</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1399,15 +1297,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2106753795</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>6974484918</t>
-        </is>
+      <c r="D28" t="n">
+        <v>2106753795</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6974484918</v>
       </c>
     </row>
     <row r="29">
@@ -1426,15 +1320,11 @@
           <t>Γενικός Ιατρός – Παθολόγος - Γηρίατρος – Γεροντολόγος - Wheelchair Accessible</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2106745205</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>6980351683</t>
-        </is>
+      <c r="D29" t="n">
+        <v>2106745205</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6980351683</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1459,15 +1349,11 @@
           <t>Ειδικός Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2810220570</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>6947328410</t>
-        </is>
+      <c r="D30" t="n">
+        <v>2810220570</v>
+      </c>
+      <c r="E30" t="n">
+        <v>6947328410</v>
       </c>
     </row>
     <row r="31">
@@ -1487,10 +1373,8 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2106890513</t>
-        </is>
+      <c r="D31" t="n">
+        <v>2106890513</v>
       </c>
     </row>
     <row r="32">
@@ -1510,10 +1394,8 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2106834141</t>
-        </is>
+      <c r="D32" t="n">
+        <v>2106834141</v>
       </c>
     </row>
     <row r="33">
@@ -1533,10 +1415,8 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2106000611</t>
-        </is>
+      <c r="D33" t="n">
+        <v>2106000611</v>
       </c>
     </row>
     <row r="34">
@@ -1555,15 +1435,11 @@
           <t>Επισκέψεις κατ’ οίκον Ηλεκτροκαρδιογραφήματος - Τοποθέτηση Καθετήρων Αναρρόφησης Εκκρίσεων - 'Ελεγχος Κολοστομίας Τραχειοστομίας - Ενδοφλέβια Ένεση - Ενδοφλέβια ΧορΉγηση Φαρμάκων Μέσω Άλλου Φλεβοκαθετήρα</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>2108002495</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>6977325007</t>
-        </is>
+      <c r="D34" t="n">
+        <v>2108002495</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6977325007</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1588,10 +1464,8 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>2106856106</t>
-        </is>
+      <c r="D35" t="n">
+        <v>2106856106</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1615,10 +1489,8 @@
           <t>Ειδικός Παθολόγος Στρατιωτικός Ιατρός</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>2107717107</t>
-        </is>
+      <c r="D36" t="n">
+        <v>2107717107</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1648,15 +1520,11 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>2106746264</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>6941499153</t>
-        </is>
+      <c r="D37" t="n">
+        <v>2106746264</v>
+      </c>
+      <c r="E37" t="n">
+        <v>6941499153</v>
       </c>
     </row>
     <row r="38">
@@ -1675,15 +1543,11 @@
           <t>Ειδικός Παθολόγος - Διδάκτωρ Πανεπιστημίου Αθηνών - Μέλος Ελληνικής Εταιρείας Υπέρτασης - Πιστοποιημένος Ιατρός Στην Ηλεκτρονική Συνταγογράφηση - Σύμβαση Με Υπουργείο Μεταφορών &amp; Ταμείο Τραπέζης Ελλάδος ΑΤΠΣΥΤΕ</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2106838647</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>6972246373</t>
-        </is>
+      <c r="D38" t="n">
+        <v>2106838647</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6972246373</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1708,10 +1572,8 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>2106756420</t>
-        </is>
+      <c r="D39" t="n">
+        <v>2106756420</v>
       </c>
     </row>
     <row r="40">
@@ -1730,15 +1592,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>2108311063</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>6974115341</t>
-        </is>
+      <c r="D40" t="n">
+        <v>2108311063</v>
+      </c>
+      <c r="E40" t="n">
+        <v>6974115341</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1763,10 +1621,8 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>2106754422</t>
-        </is>
+      <c r="D41" t="n">
+        <v>2106754422</v>
       </c>
     </row>
     <row r="42">
@@ -1786,10 +1642,8 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>2106000757</t>
-        </is>
+      <c r="D42" t="n">
+        <v>2106000757</v>
       </c>
     </row>
     <row r="43">
@@ -1809,15 +1663,11 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>2106826514</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>6944281011</t>
-        </is>
+      <c r="D43" t="n">
+        <v>2106826514</v>
+      </c>
+      <c r="E43" t="n">
+        <v>6944281011</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1842,10 +1692,8 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>2106724944</t>
-        </is>
+      <c r="D44" t="n">
+        <v>2106724944</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -1869,15 +1717,11 @@
           <t>Ειδικός Ορθοδοντικός - Ορθοδοντική Παιδιών &amp; Ενηλίκων - Invisalign - Αόρατοι Νάρθηκες - Γλωσσικά Σιδεράκια - Προ-Ορθοδοντική - Μασελάκια</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>2102838196</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>6978875087</t>
-        </is>
+      <c r="D45" t="n">
+        <v>2102838196</v>
+      </c>
+      <c r="E45" t="n">
+        <v>6978875087</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1906,10 +1750,8 @@
           <t>Ειδικός Ορθοδοντικός Παίδων &amp; Ενηλίκων - DMD - MOrth - Γερμανία - Ηνωμένο Βασίλειο</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>2102843353</t>
-        </is>
+      <c r="D46" t="n">
+        <v>2102843353</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1934,10 +1776,8 @@
           <t>Ορθοδοντικός</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>2106817624</t>
-        </is>
+      <c r="D47" t="n">
+        <v>2106817624</v>
       </c>
     </row>
     <row r="48">
@@ -1956,15 +1796,11 @@
           <t>Ειδική Παθολόγος – Επιμελήτρια Παθολόγος Κλινικής Παθολογίας &amp; Ανοσολογίας Της Ευρωκλινικής Αθηνών</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>2106835741</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>6945592521</t>
-        </is>
+      <c r="D48" t="n">
+        <v>2106835741</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6945592521</v>
       </c>
     </row>
     <row r="49">
@@ -1983,15 +1819,11 @@
           <t>Ειδικός Παθολόγος - Διδάκτωρ Δημοκρίτειου Πανεπιστήμιου Θράκης - Κατ' Οίκον Επισκέψεις</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>2106515029</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>6948087946</t>
-        </is>
+      <c r="D49" t="n">
+        <v>2106515029</v>
+      </c>
+      <c r="E49" t="n">
+        <v>6948087946</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2015,15 +1847,11 @@
           <t>Ειδική Παθολόγος - Οικογενειακή Ιατρός - Ειδικευθείσα Σε Ελβετία - Κατ' Οίκον Επισκέψεις - Συμβεβλημένη με τον ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>2109566774</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>6970506798</t>
-        </is>
+      <c r="D50" t="n">
+        <v>2109566774</v>
+      </c>
+      <c r="E50" t="n">
+        <v>6970506798</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2047,15 +1875,11 @@
           <t>Παθολόγος - Προσωπικός Γιατρός - Συμβεβλημένη με ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>2111158777</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>6978222644</t>
-        </is>
+      <c r="D51" t="n">
+        <v>2111158777</v>
+      </c>
+      <c r="E51" t="n">
+        <v>6978222644</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2079,15 +1903,11 @@
           <t>Σακχαρώδης Διαβήτης – Δυσλιπιδαιμία – Υπέρταση – Λοιμώξεις - Παρακολούθηση Χρόνιων Νοσημάτων - Πρόληψη Καρδιαγγειακών Συμβαμάτων - Συνταγογραφία - Αναγραφή Εξετάσεων Check Up - Χορήγηση Ιατρικών Γνωματεύσεων &amp; Πιστοποιητικών Υγείας - Διερεύνηση Παθήσεων Αγνώστου Αιτιολογίας</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>2111181200</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>6981033171</t>
-        </is>
+      <c r="D52" t="n">
+        <v>2111181200</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6981033171</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2111,15 +1931,11 @@
           <t>Σακχαρώδης Διαβήτης - Αρτηριακή Υπέρταση - Υπερλιπιδαιμία - Λοιμώξεις - Χρόνιες Παθήσεις - Διαφορική Διαγνωστική &amp; Θεραπευτική Παρακολούθηση</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>2102449412</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>6974953295</t>
-        </is>
+      <c r="D53" t="n">
+        <v>2102449412</v>
+      </c>
+      <c r="E53" t="n">
+        <v>6974953295</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2143,15 +1959,11 @@
           <t>Εξειδίκευση στον Σακχαρώδη Διαβήτη &amp; την Παχυσαρκία</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>2109315648</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>6974345938</t>
-        </is>
+      <c r="D54" t="n">
+        <v>2109315648</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6974345938</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2175,15 +1987,11 @@
           <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2109591846</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>6945857491</t>
-        </is>
+      <c r="D55" t="n">
+        <v>2109591846</v>
+      </c>
+      <c r="E55" t="n">
+        <v>6945857491</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2208,10 +2016,8 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>2295054665</t>
-        </is>
+      <c r="D56" t="n">
+        <v>2295054665</v>
       </c>
     </row>
     <row r="57">
@@ -2230,15 +2036,11 @@
           <t>Ειδικός Παθολόγος - Σύμβαση με Υπουργείο Συγκοινωνιών</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2114103647</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>6972838250</t>
-        </is>
+      <c r="D57" t="n">
+        <v>2114103647</v>
+      </c>
+      <c r="E57" t="n">
+        <v>6972838250</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2262,15 +2064,11 @@
           <t>Ειδικός Παθολόγος – Ηπατολόγος – Στρατιωτικός Ιατρός</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>2109919010</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>6944414808</t>
-        </is>
+      <c r="D58" t="n">
+        <v>2109919010</v>
+      </c>
+      <c r="E58" t="n">
+        <v>6944414808</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2294,15 +2092,11 @@
           <t>Ειδικός Παθολόγος  – Υπέρταση – Σάκχαρο – Διαβήτης – Λοιμώξεις - Ιώσεις - Ρύθμιση Αρτηριακής Υπέρτασης - Ρύθμιση Σακχάρου - Κατ' Οίκον Επισκέψεις Πιστοποιημένος Για Ηλεκτρονική Συνταγογράφηση &amp; Παρακλινικές Εξετάσεις - Οξυμετρία</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>2121053500</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>6937374680</t>
-        </is>
+      <c r="D59" t="n">
+        <v>2121053500</v>
+      </c>
+      <c r="E59" t="n">
+        <v>6937374680</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2326,15 +2120,11 @@
           <t>Οικογενειακός Ιατρός - Παθολόγος - Επισκέψεις Κατ' Οίκον</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>2105014500</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>6977037641</t>
-        </is>
+      <c r="D60" t="n">
+        <v>2105014500</v>
+      </c>
+      <c r="E60" t="n">
+        <v>6977037641</v>
       </c>
     </row>
     <row r="61">
@@ -2353,15 +2143,11 @@
           <t>Ειδικός Παθολόγος - Οικογενειακός Γιατρός - Ιδιωτικό Ιατρείο - Πιστοποίηση Για Ηλεκτρονική Συνταγογράφηση Φαρμάκων Και Διαγνωστικών Εξετάσεων Μέσω ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>2109658906</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>6932632898</t>
-        </is>
+      <c r="D61" t="n">
+        <v>2109658906</v>
+      </c>
+      <c r="E61" t="n">
+        <v>6932632898</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2385,15 +2171,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>2108225065</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>6947434884</t>
-        </is>
+      <c r="D62" t="n">
+        <v>2108225065</v>
+      </c>
+      <c r="E62" t="n">
+        <v>6947434884</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2417,15 +2199,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>2102799540</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>6946369199</t>
-        </is>
+      <c r="D63" t="n">
+        <v>2102799540</v>
+      </c>
+      <c r="E63" t="n">
+        <v>6946369199</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2449,15 +2227,11 @@
           <t>Ειδικός Παθολόγος Διαβητολόγος - Πιστοποιημένος ιατρός ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>2107799566</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>6944654891</t>
-        </is>
+      <c r="D64" t="n">
+        <v>2107799566</v>
+      </c>
+      <c r="E64" t="n">
+        <v>6944654891</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2481,15 +2255,11 @@
           <t>Ειδικός Παθολόγος - Σακχαρώδης Διαβήτης - Υπέρταση - Ηπατολόγος - Ρύθμιση Λοιμώξεων -Αναιμία - Παχυσαρκία - Προληπτικός Έλεγχος - Επίσκεψη Κατόπιν Ραντεβού &amp; Κατ΄οίκον</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>2114081622</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>6947326295</t>
-        </is>
+      <c r="D65" t="n">
+        <v>2114081622</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6947326295</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2513,15 +2283,11 @@
           <t>Ιατρείο Γενικής Οικογενειακής Ιατρικής - Παροχή Ιατρικής Βοήθειας Στο Σπίτι</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>2168081782</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>6945345458</t>
-        </is>
+      <c r="D66" t="n">
+        <v>2168081782</v>
+      </c>
+      <c r="E66" t="n">
+        <v>6945345458</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2545,15 +2311,11 @@
           <t>Ειδικός Παθολόγος – Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>2106610209</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>6974016795</t>
-        </is>
+      <c r="D67" t="n">
+        <v>2106610209</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6974016795</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2577,15 +2339,11 @@
           <t>Στρατιωτικός Ιατρός - Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>2111165089</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>6941505426</t>
-        </is>
+      <c r="D68" t="n">
+        <v>2111165089</v>
+      </c>
+      <c r="E68" t="n">
+        <v>6941505426</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2609,15 +2367,11 @@
           <t>Ειδικός Παθολόγος - Οικογενειακός Γιατρός</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>2299049199</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>6977695222</t>
-        </is>
+      <c r="D69" t="n">
+        <v>2299049199</v>
+      </c>
+      <c r="E69" t="n">
+        <v>6977695222</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2641,15 +2395,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>2102855326</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>6977562551</t>
-        </is>
+      <c r="D70" t="n">
+        <v>2102855326</v>
+      </c>
+      <c r="E70" t="n">
+        <v>6977562551</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2673,10 +2423,8 @@
           <t>Ειδικός Παθολόγος &amp; Διαιτολόγος</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>6944542221</t>
-        </is>
+      <c r="D71" t="n">
+        <v>6944542221</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2700,15 +2448,11 @@
           <t>Ιατρός Ηπατολόγος</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>2108829023</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>6974661171</t>
-        </is>
+      <c r="D72" t="n">
+        <v>2108829023</v>
+      </c>
+      <c r="E72" t="n">
+        <v>6974661171</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2732,15 +2476,11 @@
           <t>Ειδικός Παθολόγος – Επιμελητής Ιατρικού Ομίλου Αθηνών</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>2106124549</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>6942409460</t>
-        </is>
+      <c r="D73" t="n">
+        <v>2106124549</v>
+      </c>
+      <c r="E73" t="n">
+        <v>6942409460</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2764,10 +2504,8 @@
           <t>Ειδικός Παθολόγος - Λοιμωξιολόγος-Επιμελητής Β΄ Παθολογικής - Λοιμωξιολογικής Κλινικής Νοσοκομείου Υγεία - Επισκέψεις Κατ' Οίκον</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>2109646114</t>
-        </is>
+      <c r="D74" t="n">
+        <v>2109646114</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2791,15 +2529,11 @@
           <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>2102930460</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>6944281772</t>
-        </is>
+      <c r="D75" t="n">
+        <v>2102930460</v>
+      </c>
+      <c r="E75" t="n">
+        <v>6944281772</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2823,15 +2557,11 @@
           <t>Παθολόγος - Ιατρός Εργασίας - Βελονιστής – Γενική Τόνωση του Οργανισμού - Παχυσαρκία - Διακοπή Καπνίσματος - Αλλεργίες - Ρευματισμοί - Άγχος -  Εγκεφαλικά Επεισόδια - Μεσοθεραπεία</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>2109646400</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>6944348562</t>
-        </is>
+      <c r="D76" t="n">
+        <v>2109646400</v>
+      </c>
+      <c r="E76" t="n">
+        <v>6944348562</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2855,15 +2585,11 @@
           <t>Ειδικός Παθολόγος - Πιστοποιημένος ΕΟΠΥΥ - Συμβεβλημένος ΕΥΔΑΠ - Θεωρήσεις Διπλωμάτων Οδήγησης - Πιστοποιητικά Υγείας</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>2102014314</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>6972190704</t>
-        </is>
+      <c r="D77" t="n">
+        <v>2102014314</v>
+      </c>
+      <c r="E77" t="n">
+        <v>6972190704</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2887,15 +2613,11 @@
           <t>Γενικός Οικογενειακός Ιατρός - 24 Ώρες Νοσηλεία Και Παροχή Ιατρικής Βοήθειας Στο Σπίτι</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>2108830727</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>6979494266</t>
-        </is>
+      <c r="D78" t="n">
+        <v>2108830727</v>
+      </c>
+      <c r="E78" t="n">
+        <v>6979494266</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2919,15 +2641,11 @@
           <t>Ειδικός Παθολόγος - Πιστοποιημένος ΕΟΠΥΥ - Συμβεβλημένος ΕΥΔΑΠ - Θεωρήσεις Διπλωμάτων Οδήγησης - Πιστοποιητικά Υγείας</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>2107482041</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>6972190704</t>
-        </is>
+      <c r="D79" t="n">
+        <v>2107482041</v>
+      </c>
+      <c r="E79" t="n">
+        <v>6972190704</v>
       </c>
     </row>
     <row r="80">
@@ -2946,15 +2664,11 @@
           <t>Παθολόγος – Αναπληρώτρια Διευθύντρια Β’ Παθολογικής Κλινικής Νοσοκομείου «ΜΗΤΕΡΑ» – Διαβήτης – Λοιμώξεις - Υπερλιπιδαιμία</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>2106148114</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>6974492510</t>
-        </is>
+      <c r="D80" t="n">
+        <v>2106148114</v>
+      </c>
+      <c r="E80" t="n">
+        <v>6974492510</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2978,15 +2692,11 @@
           <t>Ειδικός Παθολόγος - Ανανεώσεις Διπλωμάτων Οδήγησης - Βεβαιώσεις Διπλώματος Οδήγησης - Λοιμώξεις Θεραπεία Αντιμετώπιση - Σακχαρώδης Διαβήτης Υπερλιπιδαιμία - Υπέρταση Έλεγχος - Εξετάσεις Αίματος - Συνταγογράφηση Φαρμάκων - Χρόνια Νοσήματα - Πιστοποιητικά Υγείας - Βεβαιώσεις Θεωρήσεις Διπλωμάτων</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>2155255842</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>6973531577</t>
-        </is>
+      <c r="D81" t="n">
+        <v>2155255842</v>
+      </c>
+      <c r="E81" t="n">
+        <v>6973531577</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3010,10 +2720,8 @@
           <t>Ειδικός Παθολόγος - Διαβητολόγος – Καθηγητής Παθολογίας - Σακχαρώδη Διαβήτη  Ιατρικής Σχολής Πανεπιστημίου - Πιστοποιημένος ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>2117350265</t>
-        </is>
+      <c r="D82" t="n">
+        <v>2117350265</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3037,15 +2745,11 @@
           <t>Διαβητικό Πόδι - Σακχαρώδης Διαβήτης &amp; Διατροφή - Αρτηριακή Υπέρταση - Αυξημένα Λιπίδια -Δυσλιπιδαιμία – Εμβολιασμοί - Λοιμώξεις – Αλλεργίες – Οστεοπόρωση - Ψυχοσωματικά Νοσήματα</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>2299063249</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>6999440441</t>
-        </is>
+      <c r="D83" t="n">
+        <v>2299063249</v>
+      </c>
+      <c r="E83" t="n">
+        <v>6999440441</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3069,15 +2773,11 @@
           <t>Παθολόγος - Εξειδίκευση σε Σακχαρώδη Διαβήτη, Διαβητικό Πόδι, Παχυσαρκία</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>2105057277</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>6972076641</t>
-        </is>
+      <c r="D84" t="n">
+        <v>2105057277</v>
+      </c>
+      <c r="E84" t="n">
+        <v>6972076641</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3101,15 +2801,11 @@
           <t>Αναπληρωτής Διευθυντής Παθολογικής Κλινικής Metropolitan General</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>2109833368</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>6978061340</t>
-        </is>
+      <c r="D85" t="n">
+        <v>2109833368</v>
+      </c>
+      <c r="E85" t="n">
+        <v>6978061340</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3133,15 +2829,11 @@
           <t>Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>2130231610</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>6977658236</t>
-        </is>
+      <c r="D86" t="n">
+        <v>2130231610</v>
+      </c>
+      <c r="E86" t="n">
+        <v>6977658236</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3165,15 +2857,11 @@
           <t>Ιατρός Ειδικός Παθολόγος</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>2104940317</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>6978613054</t>
-        </is>
+      <c r="D87" t="n">
+        <v>2104940317</v>
+      </c>
+      <c r="E87" t="n">
+        <v>6978613054</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3197,15 +2885,11 @@
           <t>Ειδικός Παθολόγος - Διαβητολόγος</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>2109414967</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>6944900690</t>
-        </is>
+      <c r="D88" t="n">
+        <v>2109414967</v>
+      </c>
+      <c r="E88" t="n">
+        <v>6944900690</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3229,15 +2913,11 @@
           <t>Ειδικός Παθολόγος - Σύμβαση Με Το Υπουργείο Μεταφορών Για Έκδοση Πιστοποιητικών Υγείας</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>2107665604</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>6946246807</t>
-        </is>
+      <c r="D89" t="n">
+        <v>2107665604</v>
+      </c>
+      <c r="E89" t="n">
+        <v>6946246807</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3261,15 +2941,11 @@
           <t>Παθολόγος</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>2107774666</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>6972920788</t>
-        </is>
+      <c r="D90" t="n">
+        <v>2107774666</v>
+      </c>
+      <c r="E90" t="n">
+        <v>6972920788</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3293,10 +2969,8 @@
           <t>Ειδικός Παθολόγος - Εξειδικευθείς σε Υπέρταση - Διακοπή Καπνίσματος - Ηλεκτρονική Συνταγογράφηση μέσω ΕΟΠΥΥ</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>6944197808</t>
-        </is>
+      <c r="D91" t="n">
+        <v>6944197808</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3307,11 +2981,11 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ΤΡΙΑΝΤΑΦΥΛΛΟΣ Α. ΜΑΝΟΥΣΟΣ - DOCTOR PLUS</t>
-        </is>
-      </c>
-      <c r="E92" t="n">
-        <v>6977325007</v>
+          <t>egertg</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>6944197808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed chrome tabs closing
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,15 +486,11 @@
           <t>Δερματολόγος – Αφροδισιολόγος - Κλινική &amp; Αισθητική Δερματολογία - Laser</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2105149109</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6970427541</t>
-        </is>
+      <c r="D2" t="n">
+        <v>2105149109</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6970427541</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -519,15 +515,11 @@
           <t>Δερματολόγος – Αφροδισιολόγος – Επισκέψεις Κατ' Οίκον</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2102110922</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6977524030</t>
-        </is>
+      <c r="D3" t="n">
+        <v>2102110922</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6977524030</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -552,15 +544,11 @@
           <t>Κλινική Δερματολογία - Αφροδισιολογία</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2103455493</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6932351230</t>
-        </is>
+      <c r="D4" t="n">
+        <v>2103455493</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6932351230</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -568,6 +556,35 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ΜΠΑΚΑ Φ. ΦΩΤΕΙΝΗ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Αργυροπούλου 11-13, Αθήνα - Κάτω Πατήσια, 11145, ΑΤΤΙΚΗΣ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Δερματολόγος – Αφροδισιολόγος – Εφαρμογές Laser – Αισθητική Δερματολογία</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2114001851</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6932431775</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
the removeduplicates works ok for non colored cells
</commit_message>
<xml_diff>
--- a/doctor_info.xlsx
+++ b/doctor_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6660" yWindow="3165" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -442,13 +442,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.42578125" customWidth="1" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -648,6 +652,16 @@
         <is>
           <t>mailTo:konspyrop@gmail.com</t>
         </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ΧΡΟΝΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>6937036009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>